<commit_message>
Update campaign graph scales and refine workspace settings
</commit_message>
<xml_diff>
--- a/Others/Hombrew/Mechanics/DnD Hombrew Lev Progesion.xlsx
+++ b/Others/Hombrew/Mechanics/DnD Hombrew Lev Progesion.xlsx
@@ -873,12 +873,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -930,25 +948,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1258,7 +1258,7 @@
   <dimension ref="A1:Z85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,22 +1275,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="89"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="95"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="86"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="92"/>
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:21" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1310,16 +1310,16 @@
         <v>30</v>
       </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="81" t="s">
+      <c r="H2" s="89"/>
+      <c r="I2" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="83"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="89"/>
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:21" s="3" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1366,7 +1366,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="13">
-        <f>SUM(ROUND(D3+25+50,0))</f>
+        <f>SUM(ROUND(D3+75,0))</f>
         <v>175</v>
       </c>
       <c r="E4" s="22"/>
@@ -1392,7 +1392,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="13">
-        <f>SUM(ROUND(D4+25+50,0))</f>
+        <f>SUM(ROUND(D4+75,0))</f>
         <v>250</v>
       </c>
       <c r="E5" s="23"/>
@@ -1411,11 +1411,11 @@
       <c r="C6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="15">
-        <f t="shared" ref="D6:D69" si="0">SUM(ROUND(D5+25+50,0))</f>
+      <c r="D6" s="13">
+        <f>SUM(ROUND(D5+75,0))</f>
         <v>325</v>
       </c>
-      <c r="E6" s="71">
+      <c r="E6" s="74">
         <f>D7+50</f>
         <v>450</v>
       </c>
@@ -1439,10 +1439,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="13">
-        <f>SUM(ROUND(D6+25+50,0))</f>
+        <f>SUM(ROUND(D6+75,0))</f>
         <v>400</v>
       </c>
-      <c r="E7" s="72"/>
+      <c r="E7" s="75"/>
       <c r="F7" s="7"/>
       <c r="G7" s="54" t="s">
         <v>11</v>
@@ -1465,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="13">
-        <f t="shared" si="0"/>
+        <f>SUM(ROUND(D7+75,0))</f>
         <v>475</v>
       </c>
       <c r="E8" s="22"/>
@@ -1485,7 +1485,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="13">
-        <f t="shared" si="0"/>
+        <f>SUM(ROUND(D8+75,0))</f>
         <v>550</v>
       </c>
       <c r="E9" s="24"/>
@@ -1504,11 +1504,11 @@
       <c r="C10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="15">
-        <f t="shared" si="0"/>
+      <c r="D10" s="13">
+        <f>SUM(ROUND(D9+75,0))</f>
         <v>625</v>
       </c>
-      <c r="E10" s="71">
+      <c r="E10" s="74">
         <v>700</v>
       </c>
       <c r="F10" s="7"/>
@@ -1524,17 +1524,17 @@
       <c r="A11" s="49">
         <v>3</v>
       </c>
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="90">
-        <f>SUM(ROUND(D10+25+50+40,0))</f>
+      <c r="D11" s="71">
+        <f>SUM(ROUND(D10+115,0))</f>
         <v>740</v>
       </c>
-      <c r="E11" s="72"/>
+      <c r="E11" s="75"/>
       <c r="F11" s="7"/>
       <c r="G11" s="54" t="s">
         <v>12</v>
@@ -1552,9 +1552,9 @@
     </row>
     <row r="12" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="50"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="96"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="73"/>
       <c r="E12" s="25"/>
       <c r="F12" s="7"/>
       <c r="G12" s="56"/>
@@ -1567,12 +1567,12 @@
     </row>
     <row r="13" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="50"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="73" t="s">
+      <c r="B13" s="77"/>
+      <c r="C13" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="90">
-        <f>SUM(ROUND(D11+25+50+75,0))</f>
+      <c r="D13" s="71">
+        <f>SUM(ROUND(D11+150,0))</f>
         <v>890</v>
       </c>
       <c r="E13" s="26"/>
@@ -1587,9 +1587,9 @@
     </row>
     <row r="14" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="51"/>
-      <c r="B14" s="94"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="92"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="27"/>
       <c r="F14" s="7"/>
       <c r="G14" s="56"/>
@@ -1604,12 +1604,12 @@
       <c r="A15" s="49">
         <v>4</v>
       </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="75" t="s">
+      <c r="B15" s="77"/>
+      <c r="C15" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="96">
-        <f>SUM(ROUND(D13+25+50+75,0))</f>
+      <c r="D15" s="73">
+        <f>SUM(ROUND(D13+150,0))</f>
         <v>1040</v>
       </c>
       <c r="E15" s="27"/>
@@ -1630,9 +1630,9 @@
     </row>
     <row r="16" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="50"/>
-      <c r="B16" s="94"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="96"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="28"/>
       <c r="F16" s="7"/>
       <c r="G16" s="56"/>
@@ -1645,12 +1645,12 @@
     </row>
     <row r="17" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="50"/>
-      <c r="B17" s="94"/>
-      <c r="C17" s="73" t="s">
+      <c r="B17" s="77"/>
+      <c r="C17" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="90">
-        <f>SUM(ROUND(D15+25+50+75,0))</f>
+      <c r="D17" s="71">
+        <f>SUM(ROUND(D15+150,0))</f>
         <v>1190</v>
       </c>
       <c r="E17" s="29"/>
@@ -1673,9 +1673,9 @@
     </row>
     <row r="18" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="51"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="92"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="68">
         <v>1400</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="13">
-        <f>SUM(ROUND(D17+25+50+100,0))</f>
+        <f>SUM(ROUND(D17+175,0))</f>
         <v>1365</v>
       </c>
       <c r="E19" s="67"/>
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="13">
-        <f t="shared" si="0"/>
+        <f>SUM(ROUND(D19+75,0))</f>
         <v>1440</v>
       </c>
       <c r="E20" s="22"/>
@@ -1769,7 +1769,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="13">
-        <f t="shared" si="0"/>
+        <f>SUM(ROUND(D20+75,0))</f>
         <v>1515</v>
       </c>
       <c r="E21" s="24"/>
@@ -1796,8 +1796,8 @@
       <c r="C22" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="15">
-        <f t="shared" si="0"/>
+      <c r="D22" s="13">
+        <f>SUM(ROUND(D21+75,0))</f>
         <v>1590</v>
       </c>
       <c r="E22" s="66">
@@ -1824,13 +1824,13 @@
       <c r="A23" s="49">
         <v>6</v>
       </c>
-      <c r="B23" s="93" t="s">
+      <c r="B23" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="90">
+      <c r="D23" s="71">
         <f>SUM(ROUND(D22+25+50+75,0))</f>
         <v>1740</v>
       </c>
@@ -1860,9 +1860,9 @@
     </row>
     <row r="24" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="50"/>
-      <c r="B24" s="94"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="96"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="73"/>
       <c r="E24" s="25"/>
       <c r="F24" s="7"/>
       <c r="G24" s="56"/>
@@ -1883,11 +1883,11 @@
     </row>
     <row r="25" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="50"/>
-      <c r="B25" s="94"/>
-      <c r="C25" s="73" t="s">
+      <c r="B25" s="77"/>
+      <c r="C25" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="90">
+      <c r="D25" s="71">
         <f>SUM(ROUND(D23+25+50+75,0))</f>
         <v>1890</v>
       </c>
@@ -1911,9 +1911,9 @@
     </row>
     <row r="26" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="51"/>
-      <c r="B26" s="94"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="92"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="30"/>
       <c r="F26" s="7"/>
       <c r="G26" s="56"/>
@@ -1936,11 +1936,11 @@
       <c r="A27" s="63">
         <v>7</v>
       </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="75" t="s">
+      <c r="B27" s="77"/>
+      <c r="C27" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="96">
+      <c r="D27" s="73">
         <f>SUM(ROUND(D25+25+50+75,0))</f>
         <v>2040</v>
       </c>
@@ -1970,9 +1970,9 @@
     </row>
     <row r="28" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="64"/>
-      <c r="B28" s="94"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="96"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="73"/>
       <c r="E28" s="28"/>
       <c r="F28" s="7"/>
       <c r="G28" s="56"/>
@@ -1993,11 +1993,11 @@
     </row>
     <row r="29" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="64"/>
-      <c r="B29" s="94"/>
-      <c r="C29" s="73" t="s">
+      <c r="B29" s="77"/>
+      <c r="C29" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="90">
+      <c r="D29" s="71">
         <f>SUM(ROUND(D27+25+50+75,0))</f>
         <v>2190</v>
       </c>
@@ -2021,9 +2021,9 @@
     </row>
     <row r="30" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="65"/>
-      <c r="B30" s="95"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="92"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="72"/>
       <c r="E30" s="68">
         <v>2450</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D6:D69" si="0">SUM(ROUND(D31+25+50,0))</f>
         <v>2490</v>
       </c>
       <c r="E32" s="22"/>
@@ -2140,13 +2140,13 @@
       <c r="A35" s="49">
         <v>9</v>
       </c>
-      <c r="B35" s="93" t="s">
+      <c r="B35" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="75" t="s">
+      <c r="C35" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="90">
+      <c r="D35" s="71">
         <f>SUM(ROUND(D34+25+50+75,0))</f>
         <v>2790</v>
       </c>
@@ -2168,9 +2168,9 @@
     </row>
     <row r="36" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="50"/>
-      <c r="B36" s="94"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="91"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="96"/>
       <c r="E36" s="25"/>
       <c r="F36" s="7"/>
       <c r="G36" s="56"/>
@@ -2183,11 +2183,11 @@
     </row>
     <row r="37" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="50"/>
-      <c r="B37" s="94"/>
-      <c r="C37" s="73" t="s">
+      <c r="B37" s="77"/>
+      <c r="C37" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="90">
+      <c r="D37" s="71">
         <f>SUM(ROUND(D35+25+50+75,0))</f>
         <v>2940</v>
       </c>
@@ -2203,9 +2203,9 @@
     </row>
     <row r="38" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="51"/>
-      <c r="B38" s="94"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="91"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="80"/>
+      <c r="D38" s="96"/>
       <c r="E38" s="30"/>
       <c r="F38" s="7"/>
       <c r="G38" s="69"/>
@@ -2220,11 +2220,11 @@
       <c r="A39" s="49">
         <v>10</v>
       </c>
-      <c r="B39" s="94"/>
-      <c r="C39" s="75" t="s">
+      <c r="B39" s="77"/>
+      <c r="C39" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="90">
+      <c r="D39" s="71">
         <f>SUM(ROUND(D37+25+50+75,0))</f>
         <v>3090</v>
       </c>
@@ -2246,9 +2246,9 @@
     </row>
     <row r="40" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="50"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="96"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="73"/>
       <c r="E40" s="28"/>
       <c r="F40" s="7"/>
       <c r="G40" s="56"/>
@@ -2261,11 +2261,11 @@
     </row>
     <row r="41" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="50"/>
-      <c r="B41" s="94"/>
-      <c r="C41" s="73" t="s">
+      <c r="B41" s="77"/>
+      <c r="C41" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="90">
+      <c r="D41" s="71">
         <f>SUM(ROUND(D39+25+50+75,0))</f>
         <v>3240</v>
       </c>
@@ -2281,9 +2281,9 @@
     </row>
     <row r="42" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="51"/>
-      <c r="B42" s="95"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="92"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="68">
         <v>3550</v>
       </c>
@@ -2392,13 +2392,13 @@
       <c r="A47" s="49">
         <v>12</v>
       </c>
-      <c r="B47" s="93" t="s">
+      <c r="B47" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="75" t="s">
+      <c r="C47" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="90">
+      <c r="D47" s="71">
         <f>SUM(ROUND(D46+25+50+75,0))</f>
         <v>3890</v>
       </c>
@@ -2420,9 +2420,9 @@
     </row>
     <row r="48" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="50"/>
-      <c r="B48" s="94"/>
-      <c r="C48" s="76"/>
-      <c r="D48" s="91"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="96"/>
       <c r="E48" s="25"/>
       <c r="F48" s="7"/>
       <c r="G48" s="56"/>
@@ -2435,11 +2435,11 @@
     </row>
     <row r="49" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="50"/>
-      <c r="B49" s="94"/>
-      <c r="C49" s="73" t="s">
+      <c r="B49" s="77"/>
+      <c r="C49" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="90">
+      <c r="D49" s="71">
         <f>SUM(ROUND(D47+25+50+75,0))</f>
         <v>4040</v>
       </c>
@@ -2455,9 +2455,9 @@
     </row>
     <row r="50" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="51"/>
-      <c r="B50" s="94"/>
-      <c r="C50" s="74"/>
-      <c r="D50" s="91"/>
+      <c r="B50" s="77"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="96"/>
       <c r="E50" s="27"/>
       <c r="F50" s="7"/>
       <c r="G50" s="69"/>
@@ -2472,11 +2472,11 @@
       <c r="A51" s="49">
         <v>13</v>
       </c>
-      <c r="B51" s="94"/>
-      <c r="C51" s="75" t="s">
+      <c r="B51" s="77"/>
+      <c r="C51" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="90">
+      <c r="D51" s="71">
         <f>SUM(ROUND(D49+25+50+75,0))</f>
         <v>4190</v>
       </c>
@@ -2498,9 +2498,9 @@
     </row>
     <row r="52" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="50"/>
-      <c r="B52" s="94"/>
-      <c r="C52" s="76"/>
-      <c r="D52" s="96"/>
+      <c r="B52" s="77"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="73"/>
       <c r="E52" s="28"/>
       <c r="F52" s="7"/>
       <c r="G52" s="56"/>
@@ -2513,11 +2513,11 @@
     </row>
     <row r="53" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="50"/>
-      <c r="B53" s="94"/>
-      <c r="C53" s="73" t="s">
+      <c r="B53" s="77"/>
+      <c r="C53" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="90">
+      <c r="D53" s="71">
         <f>SUM(ROUND(D51+25+50+75,0))</f>
         <v>4340</v>
       </c>
@@ -2533,9 +2533,9 @@
     </row>
     <row r="54" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="51"/>
-      <c r="B54" s="95"/>
-      <c r="C54" s="74"/>
-      <c r="D54" s="92"/>
+      <c r="B54" s="78"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="72"/>
       <c r="E54" s="68">
         <v>4700</v>
       </c>
@@ -2683,22 +2683,22 @@
       <c r="A59" s="49">
         <v>15</v>
       </c>
-      <c r="B59" s="93" t="s">
+      <c r="B59" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="75" t="s">
+      <c r="C59" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="D59" s="90">
+      <c r="D59" s="71">
         <f>SUM(ROUND(D57+25+50+150,0))</f>
         <v>5040</v>
       </c>
       <c r="E59" s="68"/>
       <c r="F59" s="7"/>
-      <c r="G59" s="77" t="s">
+      <c r="G59" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H59" s="78"/>
+      <c r="H59" s="84"/>
       <c r="I59" s="42">
         <v>0</v>
       </c>
@@ -2724,13 +2724,13 @@
     </row>
     <row r="60" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="50"/>
-      <c r="B60" s="94"/>
-      <c r="C60" s="76"/>
-      <c r="D60" s="96"/>
+      <c r="B60" s="77"/>
+      <c r="C60" s="82"/>
+      <c r="D60" s="73"/>
       <c r="E60" s="25"/>
       <c r="F60" s="7"/>
-      <c r="G60" s="77"/>
-      <c r="H60" s="78"/>
+      <c r="G60" s="83"/>
+      <c r="H60" s="84"/>
       <c r="I60" s="44"/>
       <c r="J60" s="45"/>
       <c r="K60" s="44"/>
@@ -2752,18 +2752,18 @@
     </row>
     <row r="61" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="50"/>
-      <c r="B61" s="94"/>
-      <c r="C61" s="73" t="s">
+      <c r="B61" s="77"/>
+      <c r="C61" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="90">
+      <c r="D61" s="71">
         <f>SUM(ROUND(D59+25+50-10,0))</f>
         <v>5105</v>
       </c>
       <c r="E61" s="34"/>
       <c r="F61" s="7"/>
-      <c r="G61" s="77"/>
-      <c r="H61" s="78"/>
+      <c r="G61" s="83"/>
+      <c r="H61" s="84"/>
       <c r="I61" s="44"/>
       <c r="J61" s="45"/>
       <c r="K61" s="44"/>
@@ -2785,13 +2785,13 @@
     </row>
     <row r="62" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="51"/>
-      <c r="B62" s="94"/>
-      <c r="C62" s="74"/>
-      <c r="D62" s="96"/>
+      <c r="B62" s="77"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="73"/>
       <c r="E62" s="30"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="79"/>
-      <c r="H62" s="80"/>
+      <c r="G62" s="85"/>
+      <c r="H62" s="86"/>
       <c r="I62" s="46"/>
       <c r="J62" s="47"/>
       <c r="K62" s="46"/>
@@ -2815,11 +2815,11 @@
       <c r="A63" s="49">
         <v>16</v>
       </c>
-      <c r="B63" s="94"/>
-      <c r="C63" s="75" t="s">
+      <c r="B63" s="77"/>
+      <c r="C63" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="90">
+      <c r="D63" s="71">
         <f>SUM(ROUND(D61+25+50+75+85,0))</f>
         <v>5340</v>
       </c>
@@ -2848,9 +2848,9 @@
     </row>
     <row r="64" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="50"/>
-      <c r="B64" s="94"/>
-      <c r="C64" s="76"/>
-      <c r="D64" s="96"/>
+      <c r="B64" s="77"/>
+      <c r="C64" s="82"/>
+      <c r="D64" s="73"/>
       <c r="E64" s="27"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
@@ -2876,11 +2876,11 @@
     </row>
     <row r="65" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="50"/>
-      <c r="B65" s="94"/>
-      <c r="C65" s="73" t="s">
+      <c r="B65" s="77"/>
+      <c r="C65" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="90">
+      <c r="D65" s="71">
         <f>SUM(ROUND(D63+25+50+75,0))</f>
         <v>5490</v>
       </c>
@@ -2909,9 +2909,9 @@
     </row>
     <row r="66" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="51"/>
-      <c r="B66" s="95"/>
-      <c r="C66" s="74"/>
-      <c r="D66" s="96"/>
+      <c r="B66" s="78"/>
+      <c r="C66" s="80"/>
+      <c r="D66" s="73"/>
       <c r="E66" s="68">
         <v>5900</v>
       </c>
@@ -3079,13 +3079,13 @@
       <c r="A71" s="49">
         <v>18</v>
       </c>
-      <c r="B71" s="93" t="s">
+      <c r="B71" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="C71" s="75" t="s">
+      <c r="C71" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="D71" s="90">
+      <c r="D71" s="71">
         <f>SUM(ROUND(D69+25+50+75,0))</f>
         <v>6165</v>
       </c>
@@ -3114,9 +3114,9 @@
     </row>
     <row r="72" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="50"/>
-      <c r="B72" s="94"/>
-      <c r="C72" s="76"/>
-      <c r="D72" s="96"/>
+      <c r="B72" s="77"/>
+      <c r="C72" s="82"/>
+      <c r="D72" s="73"/>
       <c r="E72" s="25"/>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
@@ -3142,11 +3142,11 @@
     </row>
     <row r="73" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="50"/>
-      <c r="B73" s="94"/>
-      <c r="C73" s="73" t="s">
+      <c r="B73" s="77"/>
+      <c r="C73" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="D73" s="90">
+      <c r="D73" s="71">
         <f>SUM(ROUND(D71+25+50+75,0))</f>
         <v>6315</v>
       </c>
@@ -3175,9 +3175,9 @@
     </row>
     <row r="74" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="51"/>
-      <c r="B74" s="94"/>
-      <c r="C74" s="74"/>
-      <c r="D74" s="96"/>
+      <c r="B74" s="77"/>
+      <c r="C74" s="80"/>
+      <c r="D74" s="73"/>
       <c r="E74" s="27"/>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
@@ -3205,11 +3205,11 @@
       <c r="A75" s="50">
         <v>19</v>
       </c>
-      <c r="B75" s="94"/>
-      <c r="C75" s="75" t="s">
+      <c r="B75" s="77"/>
+      <c r="C75" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D75" s="90">
+      <c r="D75" s="71">
         <f>SUM(ROUND(D73+25+50+75,0))</f>
         <v>6465</v>
       </c>
@@ -3238,9 +3238,9 @@
     </row>
     <row r="76" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="50"/>
-      <c r="B76" s="94"/>
-      <c r="C76" s="76"/>
-      <c r="D76" s="96"/>
+      <c r="B76" s="77"/>
+      <c r="C76" s="82"/>
+      <c r="D76" s="73"/>
       <c r="E76" s="39"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
@@ -3266,11 +3266,11 @@
     </row>
     <row r="77" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="50"/>
-      <c r="B77" s="94"/>
-      <c r="C77" s="73" t="s">
+      <c r="B77" s="77"/>
+      <c r="C77" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D77" s="90">
+      <c r="D77" s="71">
         <f>SUM(ROUND(D75+25+50+75,0))</f>
         <v>6615</v>
       </c>
@@ -3299,9 +3299,9 @@
     </row>
     <row r="78" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="50"/>
-      <c r="B78" s="95"/>
-      <c r="C78" s="74"/>
-      <c r="D78" s="92"/>
+      <c r="B78" s="78"/>
+      <c r="C78" s="80"/>
+      <c r="D78" s="72"/>
       <c r="E78" s="68">
         <v>7100</v>
       </c>

</xml_diff>

<commit_message>
en storm island ark nvrnght campaign, avance of the lev progresion
</commit_message>
<xml_diff>
--- a/Others/Hombrew/Mechanics/DnD Hombrew Lev Progesion.xlsx
+++ b/Others/Hombrew/Mechanics/DnD Hombrew Lev Progesion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="24240" windowHeight="13110"/>
@@ -11,7 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -786,6 +786,99 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,6 +900,18 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -816,140 +921,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1258,7 +1258,7 @@
   <dimension ref="A1:Z85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="D23" sqref="D23:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,22 +1275,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="95"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="90" t="s">
+      <c r="G1" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="92"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="48"/>
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:21" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1310,23 +1310,23 @@
         <v>30</v>
       </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="87" t="s">
+      <c r="G2" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="89"/>
-      <c r="I2" s="87" t="s">
+      <c r="H2" s="69"/>
+      <c r="I2" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="89"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="69"/>
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:21" s="3" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="49">
+      <c r="A3" s="84">
         <v>1</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="87" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -1339,16 +1339,16 @@
         <v>100</v>
       </c>
       <c r="F3" s="7"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="52" t="s">
+      <c r="G3" s="93"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="52" t="s">
+      <c r="J3" s="94"/>
+      <c r="K3" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="53"/>
+      <c r="L3" s="94"/>
       <c r="M3" s="11"/>
       <c r="N3"/>
       <c r="O3"/>
@@ -1360,13 +1360,13 @@
       <c r="U3"/>
     </row>
     <row r="4" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="50"/>
-      <c r="B4" s="61"/>
+      <c r="A4" s="85"/>
+      <c r="B4" s="88"/>
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="13">
-        <f>SUM(ROUND(D3+75,0))</f>
+        <f t="shared" ref="D4:D10" si="0">SUM(ROUND(D3+75,0))</f>
         <v>175</v>
       </c>
       <c r="E4" s="22"/>
@@ -1375,203 +1375,203 @@
         <v>14</v>
       </c>
       <c r="H4" s="55"/>
-      <c r="I4" s="42">
+      <c r="I4" s="73">
         <v>1</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="42">
+      <c r="J4" s="74"/>
+      <c r="K4" s="73">
         <v>1</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="74"/>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="50"/>
-      <c r="B5" s="61"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="88"/>
       <c r="C5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="13">
-        <f>SUM(ROUND(D4+75,0))</f>
+        <f t="shared" si="0"/>
         <v>250</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="7"/>
       <c r="G5" s="56"/>
       <c r="H5" s="57"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="45"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="76"/>
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="51"/>
-      <c r="B6" s="62"/>
+      <c r="A6" s="86"/>
+      <c r="B6" s="89"/>
       <c r="C6" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="13">
-        <f>SUM(ROUND(D5+75,0))</f>
+        <f t="shared" si="0"/>
         <v>325</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="80">
         <f>D7+50</f>
         <v>450</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="56"/>
       <c r="H6" s="57"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="47"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="78"/>
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="49">
+      <c r="A7" s="84">
         <v>2</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="87" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="13">
-        <f>SUM(ROUND(D6+75,0))</f>
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="E7" s="75"/>
+      <c r="E7" s="81"/>
       <c r="F7" s="7"/>
       <c r="G7" s="54" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="55"/>
-      <c r="I7" s="48">
+      <c r="I7" s="79">
         <v>0.8</v>
       </c>
-      <c r="J7" s="45"/>
-      <c r="K7" s="58">
+      <c r="J7" s="76"/>
+      <c r="K7" s="95">
         <v>1</v>
       </c>
-      <c r="L7" s="45"/>
+      <c r="L7" s="76"/>
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="B8" s="61"/>
+      <c r="A8" s="85"/>
+      <c r="B8" s="88"/>
       <c r="C8" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="13">
-        <f>SUM(ROUND(D7+75,0))</f>
+        <f t="shared" si="0"/>
         <v>475</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="7"/>
       <c r="G8" s="56"/>
       <c r="H8" s="57"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="45"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="76"/>
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="61"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="13">
-        <f>SUM(ROUND(D8+75,0))</f>
+        <f t="shared" si="0"/>
         <v>550</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="7"/>
       <c r="G9" s="56"/>
       <c r="H9" s="57"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="45"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="76"/>
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="62"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="89"/>
       <c r="C10" s="16" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="13">
-        <f>SUM(ROUND(D9+75,0))</f>
+        <f t="shared" si="0"/>
         <v>625</v>
       </c>
-      <c r="E10" s="74">
+      <c r="E10" s="80">
         <v>700</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="56"/>
       <c r="H10" s="57"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="45"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="76"/>
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="49">
+      <c r="A11" s="84">
         <v>3</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="71">
+      <c r="D11" s="42">
         <f>SUM(ROUND(D10+115,0))</f>
         <v>740</v>
       </c>
-      <c r="E11" s="75"/>
+      <c r="E11" s="81"/>
       <c r="F11" s="7"/>
       <c r="G11" s="54" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="55"/>
-      <c r="I11" s="42">
+      <c r="I11" s="73">
         <v>0.5</v>
       </c>
-      <c r="J11" s="43"/>
-      <c r="K11" s="42">
+      <c r="J11" s="74"/>
+      <c r="K11" s="73">
         <v>1</v>
       </c>
-      <c r="L11" s="43"/>
+      <c r="L11" s="74"/>
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="50"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="73"/>
+      <c r="A12" s="85"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="43"/>
       <c r="E12" s="25"/>
       <c r="F12" s="7"/>
       <c r="G12" s="56"/>
       <c r="H12" s="57"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="45"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="76"/>
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="50"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="79" t="s">
+      <c r="A13" s="85"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="71">
+      <c r="D13" s="42">
         <f>SUM(ROUND(D11+150,0))</f>
         <v>890</v>
       </c>
@@ -1579,36 +1579,36 @@
       <c r="F13" s="7"/>
       <c r="G13" s="56"/>
       <c r="H13" s="57"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="45"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="76"/>
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="51"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="72"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="27"/>
       <c r="F14" s="7"/>
       <c r="G14" s="56"/>
       <c r="H14" s="57"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="47"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="78"/>
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="49">
+      <c r="A15" s="84">
         <v>4</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="81" t="s">
+      <c r="B15" s="71"/>
+      <c r="C15" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="73">
+      <c r="D15" s="43">
         <f>SUM(ROUND(D13+150,0))</f>
         <v>1040</v>
       </c>
@@ -1618,38 +1618,38 @@
         <v>13</v>
       </c>
       <c r="H15" s="55"/>
-      <c r="I15" s="48">
+      <c r="I15" s="79">
         <v>0.5</v>
       </c>
-      <c r="J15" s="45"/>
-      <c r="K15" s="48">
+      <c r="J15" s="76"/>
+      <c r="K15" s="79">
         <v>1</v>
       </c>
-      <c r="L15" s="45"/>
+      <c r="L15" s="76"/>
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:21" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="73"/>
+      <c r="A16" s="85"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="43"/>
       <c r="E16" s="28"/>
       <c r="F16" s="7"/>
       <c r="G16" s="56"/>
       <c r="H16" s="57"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="45"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="76"/>
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="50"/>
-      <c r="B17" s="77"/>
-      <c r="C17" s="79" t="s">
+      <c r="A17" s="85"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="71">
+      <c r="D17" s="42">
         <f>SUM(ROUND(D15+150,0))</f>
         <v>1190</v>
       </c>
@@ -1657,10 +1657,10 @@
       <c r="F17" s="7"/>
       <c r="G17" s="56"/>
       <c r="H17" s="57"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="45"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="76"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="76"/>
       <c r="M17" s="17"/>
       <c r="N17"/>
       <c r="O17"/>
@@ -1672,20 +1672,20 @@
       <c r="U17"/>
     </row>
     <row r="18" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="51"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="68">
+      <c r="A18" s="86"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="60">
         <v>1400</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="56"/>
       <c r="H18" s="57"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="45"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="76"/>
       <c r="M18" s="7"/>
       <c r="N18"/>
       <c r="O18"/>
@@ -1697,10 +1697,10 @@
       <c r="U18"/>
     </row>
     <row r="19" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="49">
+      <c r="A19" s="84">
         <v>5</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="87" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -1710,20 +1710,20 @@
         <f>SUM(ROUND(D17+175,0))</f>
         <v>1365</v>
       </c>
-      <c r="E19" s="67"/>
+      <c r="E19" s="82"/>
       <c r="F19" s="7"/>
       <c r="G19" s="54" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="55"/>
-      <c r="I19" s="42">
+      <c r="I19" s="73">
         <v>0.4</v>
       </c>
-      <c r="J19" s="43"/>
-      <c r="K19" s="42">
+      <c r="J19" s="74"/>
+      <c r="K19" s="73">
         <v>0.9</v>
       </c>
-      <c r="L19" s="43"/>
+      <c r="L19" s="74"/>
       <c r="M19" s="7"/>
       <c r="N19"/>
       <c r="O19"/>
@@ -1735,8 +1735,8 @@
       <c r="U19"/>
     </row>
     <row r="20" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="50"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="85"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="12" t="s">
         <v>1</v>
       </c>
@@ -1748,10 +1748,10 @@
       <c r="F20" s="7"/>
       <c r="G20" s="56"/>
       <c r="H20" s="57"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="45"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="76"/>
       <c r="M20" s="7"/>
       <c r="N20"/>
       <c r="O20"/>
@@ -1763,8 +1763,8 @@
       <c r="U20"/>
     </row>
     <row r="21" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="50"/>
-      <c r="B21" s="61"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="88"/>
       <c r="C21" s="12" t="s">
         <v>2</v>
       </c>
@@ -1776,10 +1776,10 @@
       <c r="F21" s="7"/>
       <c r="G21" s="56"/>
       <c r="H21" s="57"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="45"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="76"/>
       <c r="M21" s="7"/>
       <c r="N21"/>
       <c r="O21"/>
@@ -1791,8 +1791,8 @@
       <c r="U21"/>
     </row>
     <row r="22" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="51"/>
-      <c r="B22" s="62"/>
+      <c r="A22" s="86"/>
+      <c r="B22" s="89"/>
       <c r="C22" s="14" t="s">
         <v>3</v>
       </c>
@@ -1800,16 +1800,16 @@
         <f>SUM(ROUND(D21+75,0))</f>
         <v>1590</v>
       </c>
-      <c r="E22" s="66">
+      <c r="E22" s="83">
         <v>1700</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="56"/>
       <c r="H22" s="57"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="47"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="77"/>
+      <c r="L22" s="78"/>
       <c r="M22" s="7"/>
       <c r="N22"/>
       <c r="O22"/>
@@ -1821,33 +1821,33 @@
       <c r="U22"/>
     </row>
     <row r="23" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="49">
+      <c r="A23" s="84">
         <v>6</v>
       </c>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="71">
+      <c r="D23" s="42">
         <f>SUM(ROUND(D22+25+50+75,0))</f>
         <v>1740</v>
       </c>
-      <c r="E23" s="67"/>
+      <c r="E23" s="82"/>
       <c r="F23" s="7"/>
       <c r="G23" s="54" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="55"/>
-      <c r="I23" s="48">
+      <c r="I23" s="79">
         <v>0.2</v>
       </c>
-      <c r="J23" s="45"/>
-      <c r="K23" s="48">
+      <c r="J23" s="76"/>
+      <c r="K23" s="79">
         <v>0.9</v>
       </c>
-      <c r="L23" s="45"/>
+      <c r="L23" s="76"/>
       <c r="M23" s="7"/>
       <c r="N23"/>
       <c r="O23"/>
@@ -1859,18 +1859,18 @@
       <c r="U23"/>
     </row>
     <row r="24" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="50"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="73"/>
+      <c r="A24" s="85"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="25"/>
       <c r="F24" s="7"/>
       <c r="G24" s="56"/>
       <c r="H24" s="57"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="45"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="76"/>
       <c r="M24" s="7"/>
       <c r="N24"/>
       <c r="O24"/>
@@ -1882,12 +1882,12 @@
       <c r="U24"/>
     </row>
     <row r="25" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="50"/>
-      <c r="B25" s="77"/>
-      <c r="C25" s="79" t="s">
+      <c r="A25" s="85"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="71">
+      <c r="D25" s="42">
         <f>SUM(ROUND(D23+25+50+75,0))</f>
         <v>1890</v>
       </c>
@@ -1895,10 +1895,10 @@
       <c r="F25" s="7"/>
       <c r="G25" s="56"/>
       <c r="H25" s="57"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="45"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="76"/>
       <c r="M25" s="7"/>
       <c r="N25"/>
       <c r="O25"/>
@@ -1910,18 +1910,18 @@
       <c r="U25"/>
     </row>
     <row r="26" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="51"/>
-      <c r="B26" s="77"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="72"/>
+      <c r="A26" s="86"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="44"/>
       <c r="E26" s="30"/>
       <c r="F26" s="7"/>
       <c r="G26" s="56"/>
       <c r="H26" s="57"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="45"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="76"/>
       <c r="M26" s="7"/>
       <c r="N26"/>
       <c r="O26"/>
@@ -1933,14 +1933,14 @@
       <c r="U26"/>
     </row>
     <row r="27" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="63">
+      <c r="A27" s="90">
         <v>7</v>
       </c>
-      <c r="B27" s="77"/>
-      <c r="C27" s="81" t="s">
+      <c r="B27" s="71"/>
+      <c r="C27" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="73">
+      <c r="D27" s="43">
         <f>SUM(ROUND(D25+25+50+75,0))</f>
         <v>2040</v>
       </c>
@@ -1950,14 +1950,14 @@
         <v>17</v>
       </c>
       <c r="H27" s="55"/>
-      <c r="I27" s="42">
+      <c r="I27" s="73">
         <v>0.1</v>
       </c>
-      <c r="J27" s="43"/>
-      <c r="K27" s="42">
+      <c r="J27" s="74"/>
+      <c r="K27" s="73">
         <v>0.8</v>
       </c>
-      <c r="L27" s="43"/>
+      <c r="L27" s="74"/>
       <c r="M27" s="7"/>
       <c r="N27"/>
       <c r="O27"/>
@@ -1969,18 +1969,18 @@
       <c r="U27"/>
     </row>
     <row r="28" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="64"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="73"/>
+      <c r="A28" s="91"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="43"/>
       <c r="E28" s="28"/>
       <c r="F28" s="7"/>
       <c r="G28" s="56"/>
       <c r="H28" s="57"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="45"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="76"/>
       <c r="M28" s="7"/>
       <c r="N28"/>
       <c r="O28"/>
@@ -1992,12 +1992,12 @@
       <c r="U28"/>
     </row>
     <row r="29" spans="1:21" s="1" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="64"/>
-      <c r="B29" s="77"/>
-      <c r="C29" s="79" t="s">
+      <c r="A29" s="91"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="71">
+      <c r="D29" s="42">
         <f>SUM(ROUND(D27+25+50+75,0))</f>
         <v>2190</v>
       </c>
@@ -2005,10 +2005,10 @@
       <c r="F29" s="7"/>
       <c r="G29" s="56"/>
       <c r="H29" s="57"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="45"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="76"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="76"/>
       <c r="M29" s="7"/>
       <c r="N29"/>
       <c r="O29"/>
@@ -2020,20 +2020,20 @@
       <c r="U29"/>
     </row>
     <row r="30" spans="1:21" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="65"/>
-      <c r="B30" s="78"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="68">
+      <c r="A30" s="92"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="60">
         <v>2450</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="56"/>
       <c r="H30" s="57"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="47"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="78"/>
       <c r="M30" s="7"/>
       <c r="N30"/>
       <c r="O30"/>
@@ -2045,10 +2045,10 @@
       <c r="U30"/>
     </row>
     <row r="31" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="49">
+      <c r="A31" s="84">
         <v>8</v>
       </c>
-      <c r="B31" s="60" t="s">
+      <c r="B31" s="87" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -2058,136 +2058,136 @@
         <f>SUM(ROUND(D29+25+50+150,0))</f>
         <v>2415</v>
       </c>
-      <c r="E31" s="67"/>
+      <c r="E31" s="82"/>
       <c r="F31" s="7"/>
       <c r="G31" s="54" t="s">
         <v>18</v>
       </c>
       <c r="H31" s="55"/>
-      <c r="I31" s="48">
+      <c r="I31" s="79">
         <v>0</v>
       </c>
-      <c r="J31" s="45"/>
-      <c r="K31" s="48">
+      <c r="J31" s="76"/>
+      <c r="K31" s="79">
         <v>0.7</v>
       </c>
-      <c r="L31" s="45"/>
+      <c r="L31" s="76"/>
       <c r="M31" s="4"/>
     </row>
     <row r="32" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="50"/>
-      <c r="B32" s="61"/>
+      <c r="A32" s="85"/>
+      <c r="B32" s="88"/>
       <c r="C32" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="13">
-        <f t="shared" ref="D6:D69" si="0">SUM(ROUND(D31+25+50,0))</f>
+        <f t="shared" ref="D32:D69" si="1">SUM(ROUND(D31+25+50,0))</f>
         <v>2490</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="7"/>
       <c r="G32" s="56"/>
       <c r="H32" s="57"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="45"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="76"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="76"/>
       <c r="M32" s="4"/>
     </row>
     <row r="33" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="50"/>
-      <c r="B33" s="61"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="88"/>
       <c r="C33" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2565</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="7"/>
       <c r="G33" s="56"/>
       <c r="H33" s="57"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="45"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="76"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="76"/>
       <c r="M33" s="4"/>
     </row>
     <row r="34" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="51"/>
-      <c r="B34" s="62"/>
+      <c r="A34" s="86"/>
+      <c r="B34" s="89"/>
       <c r="C34" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2640</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="83">
         <v>2800</v>
       </c>
       <c r="F34" s="7"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="45"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="76"/>
       <c r="M34" s="4"/>
     </row>
     <row r="35" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="49">
+      <c r="A35" s="84">
         <v>9</v>
       </c>
-      <c r="B35" s="76" t="s">
+      <c r="B35" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="81" t="s">
+      <c r="C35" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="71">
+      <c r="D35" s="42">
         <f>SUM(ROUND(D34+25+50+75,0))</f>
         <v>2790</v>
       </c>
-      <c r="E35" s="67"/>
+      <c r="E35" s="82"/>
       <c r="F35" s="7"/>
       <c r="G35" s="56" t="s">
         <v>19</v>
       </c>
       <c r="H35" s="57"/>
-      <c r="I35" s="42">
+      <c r="I35" s="73">
         <v>0</v>
       </c>
-      <c r="J35" s="43"/>
-      <c r="K35" s="42">
+      <c r="J35" s="74"/>
+      <c r="K35" s="73">
         <v>0.5</v>
       </c>
-      <c r="L35" s="43"/>
+      <c r="L35" s="74"/>
       <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="50"/>
-      <c r="B36" s="77"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="96"/>
+      <c r="A36" s="85"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="25"/>
       <c r="F36" s="7"/>
       <c r="G36" s="56"/>
       <c r="H36" s="57"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="45"/>
+      <c r="I36" s="75"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="75"/>
+      <c r="L36" s="76"/>
       <c r="M36" s="4"/>
     </row>
     <row r="37" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="50"/>
-      <c r="B37" s="77"/>
-      <c r="C37" s="79" t="s">
+      <c r="A37" s="85"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="71">
+      <c r="D37" s="42">
         <f>SUM(ROUND(D35+25+50+75,0))</f>
         <v>2940</v>
       </c>
@@ -2195,36 +2195,36 @@
       <c r="F37" s="7"/>
       <c r="G37" s="56"/>
       <c r="H37" s="57"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="45"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="76"/>
       <c r="M37" s="4"/>
     </row>
     <row r="38" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="51"/>
-      <c r="B38" s="77"/>
-      <c r="C38" s="80"/>
-      <c r="D38" s="96"/>
+      <c r="A38" s="86"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="45"/>
       <c r="E38" s="30"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="47"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="77"/>
+      <c r="J38" s="78"/>
+      <c r="K38" s="77"/>
+      <c r="L38" s="78"/>
       <c r="M38" s="4"/>
     </row>
     <row r="39" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="49">
+      <c r="A39" s="84">
         <v>10</v>
       </c>
-      <c r="B39" s="77"/>
-      <c r="C39" s="81" t="s">
+      <c r="B39" s="71"/>
+      <c r="C39" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="71">
+      <c r="D39" s="42">
         <f>SUM(ROUND(D37+25+50+75,0))</f>
         <v>3090</v>
       </c>
@@ -2234,38 +2234,38 @@
         <v>20</v>
       </c>
       <c r="H39" s="57"/>
-      <c r="I39" s="48">
+      <c r="I39" s="79">
         <v>0</v>
       </c>
-      <c r="J39" s="45"/>
-      <c r="K39" s="48">
+      <c r="J39" s="76"/>
+      <c r="K39" s="79">
         <v>0.5</v>
       </c>
-      <c r="L39" s="45"/>
+      <c r="L39" s="76"/>
       <c r="M39" s="4"/>
     </row>
     <row r="40" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="50"/>
-      <c r="B40" s="77"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="73"/>
+      <c r="A40" s="85"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="43"/>
       <c r="E40" s="28"/>
       <c r="F40" s="7"/>
       <c r="G40" s="56"/>
       <c r="H40" s="57"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="45"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="76"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="76"/>
       <c r="M40" s="4"/>
     </row>
     <row r="41" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="50"/>
-      <c r="B41" s="77"/>
-      <c r="C41" s="79" t="s">
+      <c r="A41" s="85"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="71">
+      <c r="D41" s="42">
         <f>SUM(ROUND(D39+25+50+75,0))</f>
         <v>3240</v>
       </c>
@@ -2273,34 +2273,34 @@
       <c r="F41" s="7"/>
       <c r="G41" s="56"/>
       <c r="H41" s="57"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="45"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="76"/>
       <c r="M41" s="4"/>
     </row>
     <row r="42" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="51"/>
-      <c r="B42" s="78"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="72"/>
-      <c r="E42" s="68">
+      <c r="A42" s="86"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="60">
         <v>3550</v>
       </c>
       <c r="F42" s="7"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="45"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="75"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="75"/>
+      <c r="L42" s="76"/>
       <c r="M42" s="4"/>
     </row>
     <row r="43" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="49">
+      <c r="A43" s="84">
         <v>11</v>
       </c>
-      <c r="B43" s="60" t="s">
+      <c r="B43" s="87" t="s">
         <v>18</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -2310,136 +2310,136 @@
         <f>SUM(ROUND(D41+25+50+200,0))</f>
         <v>3515</v>
       </c>
-      <c r="E43" s="67"/>
+      <c r="E43" s="82"/>
       <c r="F43" s="7"/>
       <c r="G43" s="56" t="s">
         <v>21</v>
       </c>
       <c r="H43" s="57"/>
-      <c r="I43" s="42">
+      <c r="I43" s="73">
         <v>0</v>
       </c>
-      <c r="J43" s="43"/>
-      <c r="K43" s="42">
+      <c r="J43" s="74"/>
+      <c r="K43" s="73">
         <v>0.4</v>
       </c>
-      <c r="L43" s="43"/>
+      <c r="L43" s="74"/>
       <c r="M43" s="4"/>
     </row>
     <row r="44" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="50"/>
-      <c r="B44" s="61"/>
+      <c r="A44" s="85"/>
+      <c r="B44" s="88"/>
       <c r="C44" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3590</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="7"/>
       <c r="G44" s="56"/>
       <c r="H44" s="57"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="45"/>
+      <c r="I44" s="75"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="75"/>
+      <c r="L44" s="76"/>
       <c r="M44" s="4"/>
     </row>
     <row r="45" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="50"/>
-      <c r="B45" s="61"/>
+      <c r="A45" s="85"/>
+      <c r="B45" s="88"/>
       <c r="C45" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D45" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3665</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="7"/>
       <c r="G45" s="56"/>
       <c r="H45" s="57"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="45"/>
+      <c r="I45" s="75"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="75"/>
+      <c r="L45" s="76"/>
       <c r="M45" s="4"/>
     </row>
     <row r="46" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="51"/>
-      <c r="B46" s="62"/>
+      <c r="A46" s="86"/>
+      <c r="B46" s="89"/>
       <c r="C46" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3740</v>
       </c>
-      <c r="E46" s="66">
+      <c r="E46" s="83">
         <v>3900</v>
       </c>
       <c r="F46" s="7"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="70"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="47"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="77"/>
+      <c r="J46" s="78"/>
+      <c r="K46" s="77"/>
+      <c r="L46" s="78"/>
       <c r="M46" s="4"/>
     </row>
     <row r="47" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="49">
+      <c r="A47" s="84">
         <v>12</v>
       </c>
-      <c r="B47" s="76" t="s">
+      <c r="B47" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="81" t="s">
+      <c r="C47" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D47" s="71">
+      <c r="D47" s="42">
         <f>SUM(ROUND(D46+25+50+75,0))</f>
         <v>3890</v>
       </c>
-      <c r="E47" s="67"/>
+      <c r="E47" s="82"/>
       <c r="F47" s="7"/>
       <c r="G47" s="54" t="s">
         <v>22</v>
       </c>
       <c r="H47" s="55"/>
-      <c r="I47" s="48">
+      <c r="I47" s="79">
         <v>0</v>
       </c>
-      <c r="J47" s="45"/>
-      <c r="K47" s="48">
+      <c r="J47" s="76"/>
+      <c r="K47" s="79">
         <v>0.4</v>
       </c>
-      <c r="L47" s="45"/>
+      <c r="L47" s="76"/>
       <c r="M47" s="4"/>
     </row>
     <row r="48" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="50"/>
-      <c r="B48" s="77"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="96"/>
+      <c r="A48" s="85"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="45"/>
       <c r="E48" s="25"/>
       <c r="F48" s="7"/>
       <c r="G48" s="56"/>
       <c r="H48" s="57"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="45"/>
-      <c r="K48" s="44"/>
-      <c r="L48" s="45"/>
+      <c r="I48" s="75"/>
+      <c r="J48" s="76"/>
+      <c r="K48" s="75"/>
+      <c r="L48" s="76"/>
       <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="50"/>
-      <c r="B49" s="77"/>
-      <c r="C49" s="79" t="s">
+      <c r="A49" s="85"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="71">
+      <c r="D49" s="42">
         <f>SUM(ROUND(D47+25+50+75,0))</f>
         <v>4040</v>
       </c>
@@ -2447,36 +2447,36 @@
       <c r="F49" s="7"/>
       <c r="G49" s="56"/>
       <c r="H49" s="57"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="44"/>
-      <c r="L49" s="45"/>
+      <c r="I49" s="75"/>
+      <c r="J49" s="76"/>
+      <c r="K49" s="75"/>
+      <c r="L49" s="76"/>
       <c r="M49" s="4"/>
     </row>
     <row r="50" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="51"/>
-      <c r="B50" s="77"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="96"/>
+      <c r="A50" s="86"/>
+      <c r="B50" s="71"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="45"/>
       <c r="E50" s="27"/>
       <c r="F50" s="7"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="45"/>
-      <c r="K50" s="44"/>
-      <c r="L50" s="45"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="75"/>
+      <c r="J50" s="76"/>
+      <c r="K50" s="75"/>
+      <c r="L50" s="76"/>
       <c r="M50" s="4"/>
     </row>
     <row r="51" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="49">
+      <c r="A51" s="84">
         <v>13</v>
       </c>
-      <c r="B51" s="77"/>
-      <c r="C51" s="81" t="s">
+      <c r="B51" s="71"/>
+      <c r="C51" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="71">
+      <c r="D51" s="42">
         <f>SUM(ROUND(D49+25+50+75,0))</f>
         <v>4190</v>
       </c>
@@ -2486,38 +2486,38 @@
         <v>23</v>
       </c>
       <c r="H51" s="57"/>
-      <c r="I51" s="42">
+      <c r="I51" s="73">
         <v>0</v>
       </c>
-      <c r="J51" s="43"/>
-      <c r="K51" s="42">
+      <c r="J51" s="74"/>
+      <c r="K51" s="73">
         <v>0.2</v>
       </c>
-      <c r="L51" s="43"/>
+      <c r="L51" s="74"/>
       <c r="M51" s="4"/>
     </row>
     <row r="52" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="50"/>
-      <c r="B52" s="77"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="73"/>
+      <c r="A52" s="85"/>
+      <c r="B52" s="71"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="43"/>
       <c r="E52" s="28"/>
       <c r="F52" s="7"/>
       <c r="G52" s="56"/>
       <c r="H52" s="57"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="45"/>
-      <c r="K52" s="44"/>
-      <c r="L52" s="45"/>
+      <c r="I52" s="75"/>
+      <c r="J52" s="76"/>
+      <c r="K52" s="75"/>
+      <c r="L52" s="76"/>
       <c r="M52" s="4"/>
     </row>
     <row r="53" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="50"/>
-      <c r="B53" s="77"/>
-      <c r="C53" s="79" t="s">
+      <c r="A53" s="85"/>
+      <c r="B53" s="71"/>
+      <c r="C53" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="71">
+      <c r="D53" s="42">
         <f>SUM(ROUND(D51+25+50+75,0))</f>
         <v>4340</v>
       </c>
@@ -2525,34 +2525,34 @@
       <c r="F53" s="7"/>
       <c r="G53" s="56"/>
       <c r="H53" s="57"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="45"/>
-      <c r="K53" s="44"/>
-      <c r="L53" s="45"/>
+      <c r="I53" s="75"/>
+      <c r="J53" s="76"/>
+      <c r="K53" s="75"/>
+      <c r="L53" s="76"/>
       <c r="M53" s="4"/>
     </row>
     <row r="54" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="51"/>
-      <c r="B54" s="78"/>
-      <c r="C54" s="80"/>
-      <c r="D54" s="72"/>
-      <c r="E54" s="68">
+      <c r="A54" s="86"/>
+      <c r="B54" s="72"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="60">
         <v>4700</v>
       </c>
       <c r="F54" s="7"/>
-      <c r="G54" s="69"/>
-      <c r="H54" s="70"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="47"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="47"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="77"/>
+      <c r="J54" s="78"/>
+      <c r="K54" s="77"/>
+      <c r="L54" s="78"/>
       <c r="M54" s="4"/>
     </row>
     <row r="55" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="49">
+      <c r="A55" s="84">
         <v>14</v>
       </c>
-      <c r="B55" s="60" t="s">
+      <c r="B55" s="87" t="s">
         <v>20</v>
       </c>
       <c r="C55" s="8" t="s">
@@ -2562,40 +2562,40 @@
         <f>SUM(ROUND(D53+25+50+250,0))</f>
         <v>4665</v>
       </c>
-      <c r="E55" s="67"/>
+      <c r="E55" s="82"/>
       <c r="F55" s="7"/>
       <c r="G55" s="56" t="s">
         <v>24</v>
       </c>
       <c r="H55" s="57"/>
-      <c r="I55" s="48">
+      <c r="I55" s="79">
         <v>0</v>
       </c>
-      <c r="J55" s="45"/>
-      <c r="K55" s="48">
+      <c r="J55" s="76"/>
+      <c r="K55" s="79">
         <v>0.1</v>
       </c>
-      <c r="L55" s="45"/>
+      <c r="L55" s="76"/>
       <c r="M55" s="4"/>
     </row>
     <row r="56" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="50"/>
-      <c r="B56" s="61"/>
+      <c r="A56" s="85"/>
+      <c r="B56" s="88"/>
       <c r="C56" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D56" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4740</v>
       </c>
       <c r="E56" s="32"/>
       <c r="F56" s="7"/>
       <c r="G56" s="56"/>
       <c r="H56" s="57"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="44"/>
-      <c r="L56" s="45"/>
+      <c r="I56" s="75"/>
+      <c r="J56" s="76"/>
+      <c r="K56" s="75"/>
+      <c r="L56" s="76"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
@@ -2612,23 +2612,23 @@
       <c r="Z56" s="4"/>
     </row>
     <row r="57" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="50"/>
-      <c r="B57" s="61"/>
+      <c r="A57" s="85"/>
+      <c r="B57" s="88"/>
       <c r="C57" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4815</v>
       </c>
       <c r="E57" s="33"/>
       <c r="F57" s="7"/>
       <c r="G57" s="56"/>
       <c r="H57" s="57"/>
-      <c r="I57" s="44"/>
-      <c r="J57" s="45"/>
-      <c r="K57" s="44"/>
-      <c r="L57" s="45"/>
+      <c r="I57" s="75"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="75"/>
+      <c r="L57" s="76"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
@@ -2645,25 +2645,25 @@
       <c r="Z57" s="4"/>
     </row>
     <row r="58" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="51"/>
-      <c r="B58" s="62"/>
+      <c r="A58" s="86"/>
+      <c r="B58" s="89"/>
       <c r="C58" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D58" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4890</v>
       </c>
-      <c r="E58" s="68">
+      <c r="E58" s="60">
         <v>5050</v>
       </c>
       <c r="F58" s="7"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="70"/>
-      <c r="I58" s="44"/>
-      <c r="J58" s="45"/>
-      <c r="K58" s="44"/>
-      <c r="L58" s="45"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="75"/>
+      <c r="J58" s="76"/>
+      <c r="K58" s="75"/>
+      <c r="L58" s="76"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
       <c r="O58" s="4"/>
@@ -2680,33 +2680,33 @@
       <c r="Z58" s="4"/>
     </row>
     <row r="59" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="49">
+      <c r="A59" s="84">
         <v>15</v>
       </c>
-      <c r="B59" s="76" t="s">
+      <c r="B59" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="81" t="s">
+      <c r="C59" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D59" s="71">
+      <c r="D59" s="42">
         <f>SUM(ROUND(D57+25+50+150,0))</f>
         <v>5040</v>
       </c>
-      <c r="E59" s="68"/>
+      <c r="E59" s="60"/>
       <c r="F59" s="7"/>
-      <c r="G59" s="83" t="s">
+      <c r="G59" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="H59" s="84"/>
-      <c r="I59" s="42">
+      <c r="H59" s="64"/>
+      <c r="I59" s="73">
         <v>0</v>
       </c>
-      <c r="J59" s="43"/>
-      <c r="K59" s="42">
+      <c r="J59" s="74"/>
+      <c r="K59" s="73">
         <v>0.01</v>
       </c>
-      <c r="L59" s="43"/>
+      <c r="L59" s="74"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
@@ -2723,18 +2723,18 @@
       <c r="Z59" s="4"/>
     </row>
     <row r="60" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="50"/>
-      <c r="B60" s="77"/>
-      <c r="C60" s="82"/>
-      <c r="D60" s="73"/>
+      <c r="A60" s="85"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="43"/>
       <c r="E60" s="25"/>
       <c r="F60" s="7"/>
-      <c r="G60" s="83"/>
-      <c r="H60" s="84"/>
-      <c r="I60" s="44"/>
-      <c r="J60" s="45"/>
-      <c r="K60" s="44"/>
-      <c r="L60" s="45"/>
+      <c r="G60" s="63"/>
+      <c r="H60" s="64"/>
+      <c r="I60" s="75"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="75"/>
+      <c r="L60" s="76"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
@@ -2751,23 +2751,23 @@
       <c r="Z60" s="4"/>
     </row>
     <row r="61" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="50"/>
-      <c r="B61" s="77"/>
-      <c r="C61" s="79" t="s">
+      <c r="A61" s="85"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="71">
+      <c r="D61" s="42">
         <f>SUM(ROUND(D59+25+50-10,0))</f>
         <v>5105</v>
       </c>
       <c r="E61" s="34"/>
       <c r="F61" s="7"/>
-      <c r="G61" s="83"/>
-      <c r="H61" s="84"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="45"/>
-      <c r="K61" s="44"/>
-      <c r="L61" s="45"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="64"/>
+      <c r="I61" s="75"/>
+      <c r="J61" s="76"/>
+      <c r="K61" s="75"/>
+      <c r="L61" s="76"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
@@ -2784,18 +2784,18 @@
       <c r="Z61" s="4"/>
     </row>
     <row r="62" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="51"/>
-      <c r="B62" s="77"/>
-      <c r="C62" s="80"/>
-      <c r="D62" s="73"/>
+      <c r="A62" s="86"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="43"/>
       <c r="E62" s="30"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="85"/>
-      <c r="H62" s="86"/>
-      <c r="I62" s="46"/>
-      <c r="J62" s="47"/>
-      <c r="K62" s="46"/>
-      <c r="L62" s="47"/>
+      <c r="G62" s="65"/>
+      <c r="H62" s="66"/>
+      <c r="I62" s="77"/>
+      <c r="J62" s="78"/>
+      <c r="K62" s="77"/>
+      <c r="L62" s="78"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
@@ -2812,14 +2812,14 @@
       <c r="Z62" s="4"/>
     </row>
     <row r="63" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="49">
+      <c r="A63" s="84">
         <v>16</v>
       </c>
-      <c r="B63" s="77"/>
-      <c r="C63" s="81" t="s">
+      <c r="B63" s="71"/>
+      <c r="C63" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="71">
+      <c r="D63" s="42">
         <f>SUM(ROUND(D61+25+50+75+85,0))</f>
         <v>5340</v>
       </c>
@@ -2847,10 +2847,10 @@
       <c r="Z63" s="4"/>
     </row>
     <row r="64" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="50"/>
-      <c r="B64" s="77"/>
-      <c r="C64" s="82"/>
-      <c r="D64" s="73"/>
+      <c r="A64" s="85"/>
+      <c r="B64" s="71"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="43"/>
       <c r="E64" s="27"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
@@ -2875,12 +2875,12 @@
       <c r="Z64" s="4"/>
     </row>
     <row r="65" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="50"/>
-      <c r="B65" s="77"/>
-      <c r="C65" s="79" t="s">
+      <c r="A65" s="85"/>
+      <c r="B65" s="71"/>
+      <c r="C65" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="71">
+      <c r="D65" s="42">
         <f>SUM(ROUND(D63+25+50+75,0))</f>
         <v>5490</v>
       </c>
@@ -2908,11 +2908,11 @@
       <c r="Z65" s="4"/>
     </row>
     <row r="66" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="51"/>
-      <c r="B66" s="78"/>
-      <c r="C66" s="80"/>
-      <c r="D66" s="73"/>
-      <c r="E66" s="68">
+      <c r="A66" s="86"/>
+      <c r="B66" s="72"/>
+      <c r="C66" s="53"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="60">
         <v>5900</v>
       </c>
       <c r="F66" s="7"/>
@@ -2938,10 +2938,10 @@
       <c r="Z66" s="4"/>
     </row>
     <row r="67" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="49">
+      <c r="A67" s="84">
         <v>17</v>
       </c>
-      <c r="B67" s="60" t="s">
+      <c r="B67" s="87" t="s">
         <v>22</v>
       </c>
       <c r="C67" s="8" t="s">
@@ -2951,7 +2951,7 @@
         <f>SUM(ROUND(D65+25+50+300,0))</f>
         <v>5865</v>
       </c>
-      <c r="E67" s="68"/>
+      <c r="E67" s="60"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
@@ -2975,13 +2975,13 @@
       <c r="Z67" s="4"/>
     </row>
     <row r="68" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="50"/>
-      <c r="B68" s="61"/>
+      <c r="A68" s="85"/>
+      <c r="B68" s="88"/>
       <c r="C68" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D68" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5940</v>
       </c>
       <c r="E68" s="36"/>
@@ -3008,13 +3008,13 @@
       <c r="Z68" s="4"/>
     </row>
     <row r="69" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="50"/>
-      <c r="B69" s="61"/>
+      <c r="A69" s="85"/>
+      <c r="B69" s="88"/>
       <c r="C69" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D69" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6015</v>
       </c>
       <c r="E69" s="37"/>
@@ -3041,16 +3041,16 @@
       <c r="Z69" s="4"/>
     </row>
     <row r="70" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="51"/>
-      <c r="B70" s="62"/>
+      <c r="A70" s="86"/>
+      <c r="B70" s="89"/>
       <c r="C70" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D70" s="15">
-        <f t="shared" ref="D70:D82" si="1">SUM(ROUND(D69+25+50,0))</f>
+        <f t="shared" ref="D70:D82" si="2">SUM(ROUND(D69+25+50,0))</f>
         <v>6090</v>
       </c>
-      <c r="E70" s="68">
+      <c r="E70" s="60">
         <v>6250</v>
       </c>
       <c r="F70" s="7"/>
@@ -3076,20 +3076,20 @@
       <c r="Z70" s="4"/>
     </row>
     <row r="71" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="49">
+      <c r="A71" s="84">
         <v>18</v>
       </c>
-      <c r="B71" s="76" t="s">
+      <c r="B71" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="C71" s="81" t="s">
+      <c r="C71" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D71" s="71">
+      <c r="D71" s="42">
         <f>SUM(ROUND(D69+25+50+75,0))</f>
         <v>6165</v>
       </c>
-      <c r="E71" s="68"/>
+      <c r="E71" s="60"/>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
@@ -3113,10 +3113,10 @@
       <c r="Z71" s="4"/>
     </row>
     <row r="72" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="50"/>
-      <c r="B72" s="77"/>
-      <c r="C72" s="82"/>
-      <c r="D72" s="73"/>
+      <c r="A72" s="85"/>
+      <c r="B72" s="71"/>
+      <c r="C72" s="62"/>
+      <c r="D72" s="43"/>
       <c r="E72" s="25"/>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
@@ -3141,12 +3141,12 @@
       <c r="Z72" s="4"/>
     </row>
     <row r="73" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="50"/>
-      <c r="B73" s="77"/>
-      <c r="C73" s="79" t="s">
+      <c r="A73" s="85"/>
+      <c r="B73" s="71"/>
+      <c r="C73" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="D73" s="71">
+      <c r="D73" s="42">
         <f>SUM(ROUND(D71+25+50+75,0))</f>
         <v>6315</v>
       </c>
@@ -3174,10 +3174,10 @@
       <c r="Z73" s="4"/>
     </row>
     <row r="74" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="51"/>
-      <c r="B74" s="77"/>
-      <c r="C74" s="80"/>
-      <c r="D74" s="73"/>
+      <c r="A74" s="86"/>
+      <c r="B74" s="71"/>
+      <c r="C74" s="53"/>
+      <c r="D74" s="43"/>
       <c r="E74" s="27"/>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
@@ -3202,14 +3202,14 @@
       <c r="Z74" s="4"/>
     </row>
     <row r="75" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="50">
+      <c r="A75" s="85">
         <v>19</v>
       </c>
-      <c r="B75" s="77"/>
-      <c r="C75" s="81" t="s">
+      <c r="B75" s="71"/>
+      <c r="C75" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D75" s="71">
+      <c r="D75" s="42">
         <f>SUM(ROUND(D73+25+50+75,0))</f>
         <v>6465</v>
       </c>
@@ -3237,10 +3237,10 @@
       <c r="Z75" s="4"/>
     </row>
     <row r="76" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="50"/>
-      <c r="B76" s="77"/>
-      <c r="C76" s="82"/>
-      <c r="D76" s="73"/>
+      <c r="A76" s="85"/>
+      <c r="B76" s="71"/>
+      <c r="C76" s="62"/>
+      <c r="D76" s="43"/>
       <c r="E76" s="39"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
@@ -3265,12 +3265,12 @@
       <c r="Z76" s="4"/>
     </row>
     <row r="77" spans="1:26" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="50"/>
-      <c r="B77" s="77"/>
-      <c r="C77" s="79" t="s">
+      <c r="A77" s="85"/>
+      <c r="B77" s="71"/>
+      <c r="C77" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D77" s="71">
+      <c r="D77" s="42">
         <f>SUM(ROUND(D75+25+50+75,0))</f>
         <v>6615</v>
       </c>
@@ -3298,11 +3298,11 @@
       <c r="Z77" s="4"/>
     </row>
     <row r="78" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="50"/>
-      <c r="B78" s="78"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="68">
+      <c r="A78" s="85"/>
+      <c r="B78" s="72"/>
+      <c r="C78" s="53"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="60">
         <v>7100</v>
       </c>
       <c r="F78" s="7"/>
@@ -3328,10 +3328,10 @@
       <c r="Z78" s="4"/>
     </row>
     <row r="79" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="49">
+      <c r="A79" s="84">
         <v>20</v>
       </c>
-      <c r="B79" s="60" t="s">
+      <c r="B79" s="87" t="s">
         <v>24</v>
       </c>
       <c r="C79" s="8" t="s">
@@ -3341,7 +3341,7 @@
         <f>SUM(ROUND(D77+25+50+350,0))</f>
         <v>7040</v>
       </c>
-      <c r="E79" s="68"/>
+      <c r="E79" s="60"/>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
@@ -3365,13 +3365,13 @@
       <c r="Z79" s="4"/>
     </row>
     <row r="80" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="50"/>
-      <c r="B80" s="61"/>
+      <c r="A80" s="85"/>
+      <c r="B80" s="88"/>
       <c r="C80" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D80" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7115</v>
       </c>
       <c r="E80" s="36"/>
@@ -3398,13 +3398,13 @@
       <c r="Z80" s="4"/>
     </row>
     <row r="81" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="50"/>
-      <c r="B81" s="61"/>
+      <c r="A81" s="85"/>
+      <c r="B81" s="88"/>
       <c r="C81" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D81" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7190</v>
       </c>
       <c r="E81" s="40"/>
@@ -3431,16 +3431,16 @@
       <c r="Z81" s="4"/>
     </row>
     <row r="82" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="51"/>
-      <c r="B82" s="62"/>
+      <c r="A82" s="86"/>
+      <c r="B82" s="89"/>
       <c r="C82" s="14" t="s">
         <v>3</v>
       </c>
       <c r="D82" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7265</v>
       </c>
-      <c r="E82" s="66">
+      <c r="E82" s="83">
         <v>20000</v>
       </c>
       <c r="F82" s="7"/>
@@ -3478,7 +3478,7 @@
       <c r="D83" s="15">
         <v>10000</v>
       </c>
-      <c r="E83" s="67"/>
+      <c r="E83" s="82"/>
       <c r="F83" s="4"/>
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
@@ -3517,22 +3517,114 @@
     </row>
   </sheetData>
   <mergeCells count="148">
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="K51:L54"/>
+    <mergeCell ref="K55:L58"/>
+    <mergeCell ref="K59:L62"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="G4:H6"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I4:J6"/>
+    <mergeCell ref="K4:L6"/>
+    <mergeCell ref="I7:J10"/>
+    <mergeCell ref="K7:L10"/>
+    <mergeCell ref="I11:J14"/>
+    <mergeCell ref="K11:L14"/>
+    <mergeCell ref="I15:J18"/>
+    <mergeCell ref="I19:J22"/>
+    <mergeCell ref="I23:J26"/>
+    <mergeCell ref="I27:J30"/>
+    <mergeCell ref="I31:J34"/>
+    <mergeCell ref="I59:J62"/>
+    <mergeCell ref="I55:J58"/>
+    <mergeCell ref="I51:J54"/>
+    <mergeCell ref="I47:J50"/>
+    <mergeCell ref="I35:J38"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="G39:H42"/>
+    <mergeCell ref="G43:H46"/>
+    <mergeCell ref="G47:H50"/>
+    <mergeCell ref="G51:H54"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="G11:H14"/>
+    <mergeCell ref="G15:H18"/>
+    <mergeCell ref="G19:H22"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B71:B78"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="G55:H58"/>
+    <mergeCell ref="G59:H62"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B59:B66"/>
+    <mergeCell ref="B47:B54"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="B11:B18"/>
+    <mergeCell ref="B23:B30"/>
+    <mergeCell ref="I43:J46"/>
+    <mergeCell ref="I39:J42"/>
+    <mergeCell ref="K15:L18"/>
+    <mergeCell ref="K19:L22"/>
+    <mergeCell ref="K23:L26"/>
+    <mergeCell ref="K27:L30"/>
+    <mergeCell ref="K35:L38"/>
+    <mergeCell ref="K31:L34"/>
+    <mergeCell ref="K39:L42"/>
+    <mergeCell ref="K43:L46"/>
+    <mergeCell ref="K47:L50"/>
+    <mergeCell ref="G7:H10"/>
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="C77:C78"/>
@@ -3557,114 +3649,22 @@
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="G55:H58"/>
-    <mergeCell ref="G59:H62"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B59:B66"/>
-    <mergeCell ref="B47:B54"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="B11:B18"/>
-    <mergeCell ref="B23:B30"/>
-    <mergeCell ref="I43:J46"/>
-    <mergeCell ref="I39:J42"/>
-    <mergeCell ref="K15:L18"/>
-    <mergeCell ref="K19:L22"/>
-    <mergeCell ref="K23:L26"/>
-    <mergeCell ref="K27:L30"/>
-    <mergeCell ref="K35:L38"/>
-    <mergeCell ref="K31:L34"/>
-    <mergeCell ref="K39:L42"/>
-    <mergeCell ref="K43:L46"/>
-    <mergeCell ref="K47:L50"/>
-    <mergeCell ref="G7:H10"/>
-    <mergeCell ref="G11:H14"/>
-    <mergeCell ref="G15:H18"/>
-    <mergeCell ref="G19:H22"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="B71:B78"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="I51:J54"/>
-    <mergeCell ref="I47:J50"/>
-    <mergeCell ref="I35:J38"/>
-    <mergeCell ref="B79:B82"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="G39:H42"/>
-    <mergeCell ref="G43:H46"/>
-    <mergeCell ref="G47:H50"/>
-    <mergeCell ref="G51:H54"/>
-    <mergeCell ref="K51:L54"/>
-    <mergeCell ref="K55:L58"/>
-    <mergeCell ref="K59:L62"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="G4:H6"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I4:J6"/>
-    <mergeCell ref="K4:L6"/>
-    <mergeCell ref="I7:J10"/>
-    <mergeCell ref="K7:L10"/>
-    <mergeCell ref="I11:J14"/>
-    <mergeCell ref="K11:L14"/>
-    <mergeCell ref="I15:J18"/>
-    <mergeCell ref="I19:J22"/>
-    <mergeCell ref="I23:J26"/>
-    <mergeCell ref="I27:J30"/>
-    <mergeCell ref="I31:J34"/>
-    <mergeCell ref="I59:J62"/>
-    <mergeCell ref="I55:J58"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D59:D60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>